<commit_message>
front changes on workflow and execution to show input-> output
</commit_message>
<xml_diff>
--- a/data/database/workflows.xlsx
+++ b/data/database/workflows.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>last_run</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -476,12 +481,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>XLSX</t>
+          <t>PDF</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>2026-01-30 10:33:11</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>EXCEL</t>
         </is>
       </c>
     </row>
@@ -501,12 +511,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Excel</t>
+          <t>EXCEL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>2026-01-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PDF</t>
         </is>
       </c>
     </row>
@@ -526,10 +541,15 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>XLSX</t>
+          <t>EXCEL</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>EXCEL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>